<commit_message>
first commit to got
</commit_message>
<xml_diff>
--- a/src/test/java/resources/TestData.xlsx
+++ b/src/test/java/resources/TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="17205" windowHeight="6615" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="17430" windowHeight="6615" firstSheet="3" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="TestCases" sheetId="1" r:id="rId1"/>
@@ -14,14 +14,15 @@
     <sheet name="ProductDetails" sheetId="4" r:id="rId5"/>
     <sheet name="SearchProduct" sheetId="6" r:id="rId6"/>
     <sheet name="AccountCreationData" sheetId="7" r:id="rId7"/>
+    <sheet name="ArticleTitle" sheetId="9" r:id="rId8"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:R7"/>
+  <oleSize ref="A1:Q20"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="121">
   <si>
     <t>TestCases</t>
   </si>
@@ -304,23 +305,98 @@
     <t>Sauce Labs Bike Light</t>
   </si>
   <si>
-    <t>testmode856+p1@gmail.com</t>
-  </si>
-  <si>
-    <t>Admin@123</t>
-  </si>
-  <si>
     <t>standard12_users</t>
   </si>
   <si>
     <t>secret_sauce123</t>
+  </si>
+  <si>
+    <t>ScenarioName</t>
+  </si>
+  <si>
+    <t>Test login with multiple credentials</t>
+  </si>
+  <si>
+    <t>Test login with invalid crdential</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ScenarioName </t>
+  </si>
+  <si>
+    <t>Validate that open product detail page functionality from product listing</t>
+  </si>
+  <si>
+    <t>Title</t>
+  </si>
+  <si>
+    <t>Lit Hub Weekly: July 7 – 11, 2025</t>
+  </si>
+  <si>
+    <t>Trump delayed his tariffs again. This could be the last time.</t>
+  </si>
+  <si>
+    <t>Trump’s trade policy brings risks for GOP, new poll shows</t>
+  </si>
+  <si>
+    <t>Blame Canada! Measles Edition</t>
+  </si>
+  <si>
+    <t>Trump threatens 30 percent tariffs on the EU, Mexico</t>
+  </si>
+  <si>
+    <t>How the GOP Regulars Won Over Donald Trump</t>
+  </si>
+  <si>
+    <t>'Huge deal': White House probe fuels speculation Trump could oust Powell</t>
+  </si>
+  <si>
+    <t>Eric Adams loses lawsuit against local election body — and his team is thrilled</t>
+  </si>
+  <si>
+    <t>State Department official defends canceling visas of pro-Palestinian academics</t>
+  </si>
+  <si>
+    <t>Federal judge blocks 'roving' immigration arrests amid Los Angeles crackdown</t>
+  </si>
+  <si>
+    <t>Trump weighs new Ukraine aid package</t>
+  </si>
+  <si>
+    <t>What Does an Obscure Urban Planning Board Have to Do With Trump’s Campaign Against Jerome Powell?</t>
+  </si>
+  <si>
+    <t>Canada pauses new tariff threats as Trump escalates</t>
+  </si>
+  <si>
+    <t>'We find another country': Homan says Trump administration looking to make deals with several countries to accept deportees.</t>
+  </si>
+  <si>
+    <t>Americans have made a U-turn on immigration since 2024 election</t>
+  </si>
+  <si>
+    <t>Trump praises FEMA response in Texas after earlier threats to eliminate agency</t>
+  </si>
+  <si>
+    <t>State lays off more than 1,300 people as Rubio pledges more efficiency</t>
+  </si>
+  <si>
+    <t>‘Alligator Alcatraz’ main architect eyes a new project: Trump’s endorsement</t>
+  </si>
+  <si>
+    <t>How Republicans’ Texas gerrymandering plan could backfire and help Dems</t>
+  </si>
+  <si>
+    <t>Global leaders’ ‘daddy’ strategy: Flatter Trump to get close to the US</t>
+  </si>
+  <si>
+    <t>Senate panel approves $500M of Ukraine aid</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -342,6 +418,18 @@
       <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF0080FF"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Consolas"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="4">
@@ -443,7 +531,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -463,6 +551,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -471,6 +563,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -824,13 +919,13 @@
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="11" t="s">
+      <c r="A4" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="B4" s="12"/>
-      <c r="C4" s="12"/>
-      <c r="D4" s="12"/>
-      <c r="E4" s="13"/>
+      <c r="B4" s="16"/>
+      <c r="C4" s="16"/>
+      <c r="D4" s="16"/>
+      <c r="E4" s="17"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
@@ -1037,10 +1132,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1052,20 +1147,26 @@
     <col min="5" max="5" width="17.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>48</v>
       </c>
       <c r="B1" s="7" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>87</v>
       </c>
       <c r="B2" t="s">
         <v>88</v>
+      </c>
+      <c r="C2" t="s">
+        <v>95</v>
       </c>
     </row>
   </sheetData>
@@ -1076,15 +1177,18 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="14" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>48</v>
       </c>
@@ -1094,19 +1198,25 @@
       <c r="C1" s="1" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" s="11" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C2" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D2" s="12" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>89</v>
       </c>
@@ -1116,9 +1226,13 @@
       <c r="C3" t="s">
         <v>90</v>
       </c>
+      <c r="D3" s="12" t="s">
+        <v>96</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1154,56 +1268,39 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection sqref="A1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="11.7109375" customWidth="1"/>
-    <col min="2" max="2" width="12.28515625" customWidth="1"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="B1" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="C1" s="7" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
-        <v>92</v>
-      </c>
-      <c r="B2" s="8" t="s">
-        <v>93</v>
-      </c>
-      <c r="C2" s="6" t="s">
+      <c r="B1" s="13" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>87</v>
-      </c>
-      <c r="B3" t="s">
-        <v>88</v>
-      </c>
-      <c r="C3" s="6" t="s">
+      <c r="B2" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
         <v>91</v>
       </c>
+      <c r="B3" s="14" t="s">
+        <v>98</v>
+      </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1"/>
-    <hyperlink ref="B2" r:id="rId2"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1454,4 +1551,130 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A22"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" s="18" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" s="18" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" s="18" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" s="18" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" s="18" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" s="18" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" s="18" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" s="18" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" s="18" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" s="18" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" s="18" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" s="18" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" s="18" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15" s="18" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16" s="18" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" s="18" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" s="18" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" s="18" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" s="18" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" s="18" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" s="18" t="s">
+        <v>120</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
this is my first commit to this project
</commit_message>
<xml_diff>
--- a/src/test/java/resources/TestData.xlsx
+++ b/src/test/java/resources/TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="17430" windowHeight="6615" firstSheet="3" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="16230" windowHeight="3780" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="TestCases" sheetId="1" r:id="rId1"/>
@@ -17,12 +17,12 @@
     <sheet name="ArticleTitle" sheetId="9" r:id="rId8"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:Q20"/>
+  <oleSize ref="A1:P11"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="123">
   <si>
     <t>TestCases</t>
   </si>
@@ -390,13 +390,19 @@
   </si>
   <si>
     <t>Senate panel approves $500M of Ukraine aid</t>
+  </si>
+  <si>
+    <t>actual</t>
+  </si>
+  <si>
+    <t>https://www.saucedemo.com/v1/inventory.html</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -428,6 +434,12 @@
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF2A00FF"/>
       <name val="Consolas"/>
       <family val="3"/>
     </font>
@@ -531,7 +543,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -555,6 +567,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -563,9 +579,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -919,13 +932,13 @@
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="15" t="s">
+      <c r="A4" s="17" t="s">
         <v>38</v>
       </c>
-      <c r="B4" s="16"/>
-      <c r="C4" s="16"/>
-      <c r="D4" s="16"/>
-      <c r="E4" s="17"/>
+      <c r="B4" s="18"/>
+      <c r="C4" s="18"/>
+      <c r="D4" s="18"/>
+      <c r="E4" s="19"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
@@ -1132,10 +1145,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1147,7 +1160,7 @@
     <col min="5" max="5" width="17.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>48</v>
       </c>
@@ -1157,8 +1170,11 @@
       <c r="C1" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>87</v>
       </c>
@@ -1168,10 +1184,13 @@
       <c r="C2" t="s">
         <v>95</v>
       </c>
+      <c r="D2" s="16" t="s">
+        <v>122</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1179,8 +1198,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1268,7 +1287,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:B1048576"/>
@@ -1276,7 +1295,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>51</v>
       </c>
@@ -1284,7 +1303,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>91</v>
       </c>
@@ -1292,7 +1311,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>91</v>
       </c>
@@ -1333,7 +1352,7 @@
   <dimension ref="A1:O4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1557,7 +1576,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:A22"/>
     </sheetView>
   </sheetViews>
@@ -1569,107 +1588,107 @@
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" s="18" t="s">
+      <c r="A2" s="15" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" s="18" t="s">
+      <c r="A3" s="15" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" s="18" t="s">
+      <c r="A4" s="15" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" s="18" t="s">
+      <c r="A5" s="15" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" s="18" t="s">
+      <c r="A6" s="15" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" s="18" t="s">
+      <c r="A7" s="15" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" s="18" t="s">
+      <c r="A8" s="15" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9" s="18" t="s">
+      <c r="A9" s="15" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A10" s="18" t="s">
+      <c r="A10" s="15" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A11" s="18" t="s">
+      <c r="A11" s="15" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A12" s="18" t="s">
+      <c r="A12" s="15" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A13" s="18" t="s">
+      <c r="A13" s="15" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A14" s="18" t="s">
+      <c r="A14" s="15" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A15" s="18" t="s">
+      <c r="A15" s="15" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A16" s="18" t="s">
+      <c r="A16" s="15" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" s="18" t="s">
+      <c r="A17" s="15" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" s="18" t="s">
+      <c r="A18" s="15" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" s="18" t="s">
+      <c r="A19" s="15" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" s="18" t="s">
+      <c r="A20" s="15" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21" s="18" t="s">
+      <c r="A21" s="15" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A22" s="18" t="s">
+      <c r="A22" s="15" t="s">
         <v>120</v>
       </c>
     </row>

</xml_diff>